<commit_message>
redid data with new sizes
</commit_message>
<xml_diff>
--- a/timing_results.xlsx
+++ b/timing_results.xlsx
@@ -526,34 +526,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3.099441528320312e-06</v>
+        <v>3.576278686523438e-06</v>
       </c>
       <c r="C2" t="n">
-        <v>5.7220458984375e-06</v>
+        <v>3.814697265625e-06</v>
       </c>
       <c r="D2" t="n">
-        <v>2.622604370117188e-06</v>
+        <v>1.192092895507812e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>1.096725463867188e-05</v>
+        <v>2.145767211914062e-06</v>
       </c>
       <c r="F2" t="n">
-        <v>3.099441528320312e-06</v>
+        <v>1.9073486328125e-06</v>
       </c>
       <c r="G2" t="n">
-        <v>2.86102294921875e-06</v>
+        <v>2.145767211914062e-06</v>
       </c>
       <c r="H2" t="n">
-        <v>2.86102294921875e-06</v>
+        <v>1.192092895507812e-06</v>
       </c>
       <c r="I2" t="n">
-        <v>1.668930053710938e-06</v>
+        <v>7.152557373046875e-07</v>
       </c>
       <c r="J2" t="n">
-        <v>1.668930053710938e-06</v>
+        <v>7.152557373046875e-07</v>
       </c>
       <c r="K2" t="n">
-        <v>1.668930053710938e-06</v>
+        <v>1.192092895507812e-06</v>
       </c>
       <c r="L2">
         <f>AVERAGE(B2:K2)</f>
@@ -566,37 +566,37 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B3" t="n">
-        <v>0.01015400886535645</v>
+        <v>0.04208827018737793</v>
       </c>
       <c r="C3" t="n">
-        <v>0.009883642196655273</v>
+        <v>0.04571247100830078</v>
       </c>
       <c r="D3" t="n">
-        <v>0.009865760803222656</v>
+        <v>0.0386815071105957</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01050829887390137</v>
+        <v>0.04149127006530762</v>
       </c>
       <c r="F3" t="n">
-        <v>0.009624958038330078</v>
+        <v>0.0389859676361084</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01097440719604492</v>
+        <v>0.04320383071899414</v>
       </c>
       <c r="H3" t="n">
-        <v>0.01027631759643555</v>
+        <v>0.03923869132995605</v>
       </c>
       <c r="I3" t="n">
-        <v>0.01231789588928223</v>
+        <v>0.03976917266845703</v>
       </c>
       <c r="J3" t="n">
-        <v>0.009759664535522461</v>
+        <v>0.04477643966674805</v>
       </c>
       <c r="K3" t="n">
-        <v>0.01007676124572754</v>
+        <v>0.04109621047973633</v>
       </c>
       <c r="L3">
         <f>AVERAGE(B3:K3)</f>
@@ -609,37 +609,37 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="B4" t="n">
-        <v>0.04054784774780273</v>
+        <v>0.1566979885101318</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03898882865905762</v>
+        <v>0.160341739654541</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04022598266601562</v>
+        <v>0.1572701930999756</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0400245189666748</v>
+        <v>0.1587464809417725</v>
       </c>
       <c r="F4" t="n">
-        <v>0.04089021682739258</v>
+        <v>0.1577141284942627</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04009819030761719</v>
+        <v>0.1605966091156006</v>
       </c>
       <c r="H4" t="n">
-        <v>0.04735779762268066</v>
+        <v>0.1619212627410889</v>
       </c>
       <c r="I4" t="n">
-        <v>0.03864073753356934</v>
+        <v>0.1600699424743652</v>
       </c>
       <c r="J4" t="n">
-        <v>0.04383635520935059</v>
+        <v>0.1562099456787109</v>
       </c>
       <c r="K4" t="n">
-        <v>0.03915691375732422</v>
+        <v>0.160663366317749</v>
       </c>
       <c r="L4">
         <f>AVERAGE(B4:K4)</f>
@@ -652,37 +652,37 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="B5" t="n">
-        <v>0.08902168273925781</v>
+        <v>0.3513696193695068</v>
       </c>
       <c r="C5" t="n">
-        <v>0.09345626831054688</v>
+        <v>0.3570907115936279</v>
       </c>
       <c r="D5" t="n">
-        <v>0.09284567832946777</v>
+        <v>0.3501062393188477</v>
       </c>
       <c r="E5" t="n">
-        <v>0.08859014511108398</v>
+        <v>0.3559532165527344</v>
       </c>
       <c r="F5" t="n">
-        <v>0.089111328125</v>
+        <v>0.3539128303527832</v>
       </c>
       <c r="G5" t="n">
-        <v>0.09234309196472168</v>
+        <v>0.3547420501708984</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09685492515563965</v>
+        <v>0.3518776893615723</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1031448841094971</v>
+        <v>0.3583123683929443</v>
       </c>
       <c r="J5" t="n">
-        <v>0.09894800186157227</v>
+        <v>0.3493270874023438</v>
       </c>
       <c r="K5" t="n">
-        <v>0.08828616142272949</v>
+        <v>0.3555731773376465</v>
       </c>
       <c r="L5">
         <f>AVERAGE(B5:K5)</f>
@@ -695,37 +695,37 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1602511405944824</v>
+        <v>0.6416592597961426</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1608576774597168</v>
+        <v>0.6862530708312988</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1702690124511719</v>
+        <v>0.6367764472961426</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1639118194580078</v>
+        <v>0.7484517097473145</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1601924896240234</v>
+        <v>0.6362960338592529</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1582720279693604</v>
+        <v>0.6355326175689697</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1607260704040527</v>
+        <v>0.6237063407897949</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1595184803009033</v>
+        <v>0.6676595211029053</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1563141345977783</v>
+        <v>0.6421687602996826</v>
       </c>
       <c r="K6" t="n">
-        <v>0.15981125831604</v>
+        <v>0.6449816226959229</v>
       </c>
       <c r="L6">
         <f>AVERAGE(B6:K6)</f>
@@ -738,37 +738,37 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="B7" t="n">
-        <v>0.248340368270874</v>
+        <v>1.028444051742554</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2389020919799805</v>
+        <v>1.009976863861084</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2474167346954346</v>
+        <v>1.027829647064209</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2463588714599609</v>
+        <v>1.065417528152466</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2386624813079834</v>
+        <v>1.044753789901733</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2466685771942139</v>
+        <v>1.029937744140625</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2503433227539062</v>
+        <v>0.9980900287628174</v>
       </c>
       <c r="I7" t="n">
-        <v>0.240607738494873</v>
+        <v>1.02228856086731</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2476844787597656</v>
+        <v>1.019595861434937</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2456009387969971</v>
+        <v>1.040081262588501</v>
       </c>
       <c r="L7">
         <f>AVERAGE(B7:K7)</f>
@@ -885,34 +885,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3.457069396972656e-05</v>
+        <v>2.980232238769531e-05</v>
       </c>
       <c r="C2" t="n">
-        <v>1.978874206542969e-05</v>
+        <v>1.33514404296875e-05</v>
       </c>
       <c r="D2" t="n">
-        <v>1.025199890136719e-05</v>
+        <v>4.76837158203125e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>1.33514404296875e-05</v>
+        <v>8.344650268554688e-06</v>
       </c>
       <c r="F2" t="n">
-        <v>1.025199890136719e-05</v>
+        <v>6.198883056640625e-06</v>
       </c>
       <c r="G2" t="n">
-        <v>9.298324584960938e-06</v>
+        <v>8.821487426757812e-06</v>
       </c>
       <c r="H2" t="n">
-        <v>1.096725463867188e-05</v>
+        <v>4.291534423828125e-06</v>
       </c>
       <c r="I2" t="n">
-        <v>6.914138793945312e-06</v>
+        <v>3.099441528320312e-06</v>
       </c>
       <c r="J2" t="n">
-        <v>8.344650268554688e-06</v>
+        <v>2.86102294921875e-06</v>
       </c>
       <c r="K2" t="n">
-        <v>6.67572021484375e-06</v>
+        <v>2.86102294921875e-06</v>
       </c>
       <c r="L2">
         <f>AVERAGE(B2:K2)</f>
@@ -925,37 +925,37 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0007956027984619141</v>
+        <v>0.001081705093383789</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0005159378051757812</v>
+        <v>0.001033782958984375</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0005996227264404297</v>
+        <v>0.0009775161743164062</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0005483627319335938</v>
+        <v>0.001008749008178711</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0006172657012939453</v>
+        <v>0.001081228256225586</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0005691051483154297</v>
+        <v>0.001187562942504883</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0005199909210205078</v>
+        <v>0.001106739044189453</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0006699562072753906</v>
+        <v>0.001053094863891602</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0005507469177246094</v>
+        <v>0.001139402389526367</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0005435943603515625</v>
+        <v>0.001062154769897461</v>
       </c>
       <c r="L3">
         <f>AVERAGE(B3:K3)</f>
@@ -968,37 +968,37 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="B4" t="n">
-        <v>0.001380443572998047</v>
+        <v>0.002152442932128906</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001066923141479492</v>
+        <v>0.002050399780273438</v>
       </c>
       <c r="D4" t="n">
-        <v>0.001112937927246094</v>
+        <v>0.00194096565246582</v>
       </c>
       <c r="E4" t="n">
-        <v>0.001070499420166016</v>
+        <v>0.001989126205444336</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0009963512420654297</v>
+        <v>0.001961231231689453</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0009772777557373047</v>
+        <v>0.002144575119018555</v>
       </c>
       <c r="H4" t="n">
-        <v>0.001030921936035156</v>
+        <v>0.002060413360595703</v>
       </c>
       <c r="I4" t="n">
-        <v>0.001033306121826172</v>
+        <v>0.002064228057861328</v>
       </c>
       <c r="J4" t="n">
-        <v>0.001142024993896484</v>
+        <v>0.002092599868774414</v>
       </c>
       <c r="K4" t="n">
-        <v>0.001027822494506836</v>
+        <v>0.001862525939941406</v>
       </c>
       <c r="L4">
         <f>AVERAGE(B4:K4)</f>
@@ -1011,37 +1011,37 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="B5" t="n">
-        <v>0.001582860946655273</v>
+        <v>0.002901315689086914</v>
       </c>
       <c r="C5" t="n">
-        <v>0.001420974731445312</v>
+        <v>0.003487348556518555</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001509189605712891</v>
+        <v>0.003481626510620117</v>
       </c>
       <c r="E5" t="n">
-        <v>0.001473665237426758</v>
+        <v>0.003158330917358398</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00170445442199707</v>
+        <v>0.002799510955810547</v>
       </c>
       <c r="G5" t="n">
-        <v>0.001443862915039062</v>
+        <v>0.002933502197265625</v>
       </c>
       <c r="H5" t="n">
-        <v>0.001471042633056641</v>
+        <v>0.002854108810424805</v>
       </c>
       <c r="I5" t="n">
-        <v>0.001420259475708008</v>
+        <v>0.002927303314208984</v>
       </c>
       <c r="J5" t="n">
-        <v>0.001494884490966797</v>
+        <v>0.002887725830078125</v>
       </c>
       <c r="K5" t="n">
-        <v>0.001540184020996094</v>
+        <v>0.002881526947021484</v>
       </c>
       <c r="L5">
         <f>AVERAGE(B5:K5)</f>
@@ -1054,37 +1054,37 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="B6" t="n">
-        <v>0.001951932907104492</v>
+        <v>0.004082441329956055</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001977920532226562</v>
+        <v>0.003956794738769531</v>
       </c>
       <c r="D6" t="n">
-        <v>0.002737998962402344</v>
+        <v>0.008474349975585938</v>
       </c>
       <c r="E6" t="n">
-        <v>0.001935720443725586</v>
+        <v>0.004492044448852539</v>
       </c>
       <c r="F6" t="n">
-        <v>0.001892566680908203</v>
+        <v>0.004628181457519531</v>
       </c>
       <c r="G6" t="n">
-        <v>0.001899957656860352</v>
+        <v>0.003955841064453125</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00194096565246582</v>
+        <v>0.003919601440429688</v>
       </c>
       <c r="I6" t="n">
-        <v>0.002297401428222656</v>
+        <v>0.004063129425048828</v>
       </c>
       <c r="J6" t="n">
-        <v>0.002135515213012695</v>
+        <v>0.004046916961669922</v>
       </c>
       <c r="K6" t="n">
-        <v>0.001898765563964844</v>
+        <v>0.003969907760620117</v>
       </c>
       <c r="L6">
         <f>AVERAGE(B6:K6)</f>
@@ -1097,37 +1097,37 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="B7" t="n">
-        <v>0.002355813980102539</v>
+        <v>0.005184173583984375</v>
       </c>
       <c r="C7" t="n">
-        <v>0.002228498458862305</v>
+        <v>0.004668235778808594</v>
       </c>
       <c r="D7" t="n">
-        <v>0.002321481704711914</v>
+        <v>0.005610227584838867</v>
       </c>
       <c r="E7" t="n">
-        <v>0.002267122268676758</v>
+        <v>0.004596471786499023</v>
       </c>
       <c r="F7" t="n">
-        <v>0.002263307571411133</v>
+        <v>0.004528045654296875</v>
       </c>
       <c r="G7" t="n">
-        <v>0.002378702163696289</v>
+        <v>0.004647016525268555</v>
       </c>
       <c r="H7" t="n">
-        <v>0.002347230911254883</v>
+        <v>0.004456996917724609</v>
       </c>
       <c r="I7" t="n">
-        <v>0.002430438995361328</v>
+        <v>0.00442957878112793</v>
       </c>
       <c r="J7" t="n">
-        <v>0.002361297607421875</v>
+        <v>0.005900859832763672</v>
       </c>
       <c r="K7" t="n">
-        <v>0.002300262451171875</v>
+        <v>0.005107402801513672</v>
       </c>
       <c r="L7">
         <f>AVERAGE(B7:K7)</f>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B3">
         <f>'Brute Force'!L3</f>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="B4">
         <f>'Brute Force'!L4</f>
@@ -1274,7 +1274,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="B5">
         <f>'Brute Force'!L5</f>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="B6">
         <f>'Brute Force'!L6</f>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="B7">
         <f>'Brute Force'!L7</f>

</xml_diff>

<commit_message>
updated code including fixed base case
</commit_message>
<xml_diff>
--- a/timing_results.xlsx
+++ b/timing_results.xlsx
@@ -526,34 +526,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3.576278686523438e-06</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>3.814697265625e-06</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1.192092895507812e-06</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2.145767211914062e-06</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1.9073486328125e-06</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2.145767211914062e-06</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1.192092895507812e-06</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>7.152557373046875e-07</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>7.152557373046875e-07</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1.192092895507812e-06</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <f>AVERAGE(B2:K2)</f>
@@ -569,34 +569,34 @@
         <v>200</v>
       </c>
       <c r="B3" t="n">
-        <v>0.04208827018737793</v>
+        <v>0.05807828903198242</v>
       </c>
       <c r="C3" t="n">
-        <v>0.04571247100830078</v>
+        <v>0.05686426162719727</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0386815071105957</v>
+        <v>0.05745244026184082</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04149127006530762</v>
+        <v>0.0593106746673584</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0389859676361084</v>
+        <v>0.05231833457946777</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04320383071899414</v>
+        <v>0.05089449882507324</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03923869132995605</v>
+        <v>0.07591700553894043</v>
       </c>
       <c r="I3" t="n">
-        <v>0.03976917266845703</v>
+        <v>0.04929590225219727</v>
       </c>
       <c r="J3" t="n">
-        <v>0.04477643966674805</v>
+        <v>0.05038046836853027</v>
       </c>
       <c r="K3" t="n">
-        <v>0.04109621047973633</v>
+        <v>0.05597138404846191</v>
       </c>
       <c r="L3">
         <f>AVERAGE(B3:K3)</f>
@@ -612,34 +612,34 @@
         <v>400</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1566979885101318</v>
+        <v>0.2040259838104248</v>
       </c>
       <c r="C4" t="n">
-        <v>0.160341739654541</v>
+        <v>0.2096037864685059</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1572701930999756</v>
+        <v>0.2194952964782715</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1587464809417725</v>
+        <v>0.2248122692108154</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1577141284942627</v>
+        <v>0.2093229293823242</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1605966091156006</v>
+        <v>0.221970796585083</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1619212627410889</v>
+        <v>0.2260551452636719</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1600699424743652</v>
+        <v>0.2072842121124268</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1562099456787109</v>
+        <v>0.2137517929077148</v>
       </c>
       <c r="K4" t="n">
-        <v>0.160663366317749</v>
+        <v>0.2056353092193604</v>
       </c>
       <c r="L4">
         <f>AVERAGE(B4:K4)</f>
@@ -655,34 +655,34 @@
         <v>600</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3513696193695068</v>
+        <v>0.4634144306182861</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3570907115936279</v>
+        <v>0.4614531993865967</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3501062393188477</v>
+        <v>0.6120820045471191</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3559532165527344</v>
+        <v>0.4511904716491699</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3539128303527832</v>
+        <v>0.4643123149871826</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3547420501708984</v>
+        <v>0.475156307220459</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3518776893615723</v>
+        <v>0.5719192028045654</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3583123683929443</v>
+        <v>0.4635899066925049</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3493270874023438</v>
+        <v>0.4749021530151367</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3555731773376465</v>
+        <v>0.4656960964202881</v>
       </c>
       <c r="L5">
         <f>AVERAGE(B5:K5)</f>
@@ -698,34 +698,34 @@
         <v>800</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6416592597961426</v>
+        <v>0.8650112152099609</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6862530708312988</v>
+        <v>0.82700514793396</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6367764472961426</v>
+        <v>0.9095418453216553</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7484517097473145</v>
+        <v>0.9233608245849609</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6362960338592529</v>
+        <v>0.8982982635498047</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6355326175689697</v>
+        <v>0.9550714492797852</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6237063407897949</v>
+        <v>0.8983595371246338</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6676595211029053</v>
+        <v>0.9080491065979004</v>
       </c>
       <c r="J6" t="n">
-        <v>0.6421687602996826</v>
+        <v>0.9102048873901367</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6449816226959229</v>
+        <v>0.9253726005554199</v>
       </c>
       <c r="L6">
         <f>AVERAGE(B6:K6)</f>
@@ -741,34 +741,34 @@
         <v>1000</v>
       </c>
       <c r="B7" t="n">
-        <v>1.028444051742554</v>
+        <v>1.434290409088135</v>
       </c>
       <c r="C7" t="n">
-        <v>1.009976863861084</v>
+        <v>1.415933132171631</v>
       </c>
       <c r="D7" t="n">
-        <v>1.027829647064209</v>
+        <v>1.590587615966797</v>
       </c>
       <c r="E7" t="n">
-        <v>1.065417528152466</v>
+        <v>1.633319854736328</v>
       </c>
       <c r="F7" t="n">
-        <v>1.044753789901733</v>
+        <v>1.539464712142944</v>
       </c>
       <c r="G7" t="n">
-        <v>1.029937744140625</v>
+        <v>1.50659441947937</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9980900287628174</v>
+        <v>1.43195104598999</v>
       </c>
       <c r="I7" t="n">
-        <v>1.02228856086731</v>
+        <v>1.413079023361206</v>
       </c>
       <c r="J7" t="n">
-        <v>1.019595861434937</v>
+        <v>1.379208087921143</v>
       </c>
       <c r="K7" t="n">
-        <v>1.040081262588501</v>
+        <v>1.407622098922729</v>
       </c>
       <c r="L7">
         <f>AVERAGE(B7:K7)</f>
@@ -885,34 +885,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2.980232238769531e-05</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.33514404296875e-05</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>4.76837158203125e-06</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>8.344650268554688e-06</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>6.198883056640625e-06</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8.821487426757812e-06</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>4.291534423828125e-06</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>3.099441528320312e-06</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>2.86102294921875e-06</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>2.86102294921875e-06</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <f>AVERAGE(B2:K2)</f>
@@ -928,34 +928,34 @@
         <v>200</v>
       </c>
       <c r="B3" t="n">
-        <v>0.001081705093383789</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.001033782958984375</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0009775161743164062</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.001008749008178711</v>
+        <v>0.005215883255004883</v>
       </c>
       <c r="F3" t="n">
-        <v>0.001081228256225586</v>
+        <v>0.008206605911254883</v>
       </c>
       <c r="G3" t="n">
-        <v>0.001187562942504883</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001106739044189453</v>
+        <v>0.00806427001953125</v>
       </c>
       <c r="I3" t="n">
-        <v>0.001053094863891602</v>
+        <v>0.006873846054077148</v>
       </c>
       <c r="J3" t="n">
-        <v>0.001139402389526367</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.001062154769897461</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <f>AVERAGE(B3:K3)</f>
@@ -971,34 +971,34 @@
         <v>400</v>
       </c>
       <c r="B4" t="n">
-        <v>0.002152442932128906</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002050399780273438</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00194096565246582</v>
+        <v>0.01570534706115723</v>
       </c>
       <c r="E4" t="n">
-        <v>0.001989126205444336</v>
+        <v>0.009578466415405273</v>
       </c>
       <c r="F4" t="n">
-        <v>0.001961231231689453</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.002144575119018555</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.002060413360595703</v>
+        <v>0.003987550735473633</v>
       </c>
       <c r="I4" t="n">
-        <v>0.002064228057861328</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.002092599868774414</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.001862525939941406</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <f>AVERAGE(B4:K4)</f>
@@ -1014,34 +1014,34 @@
         <v>600</v>
       </c>
       <c r="B5" t="n">
-        <v>0.002901315689086914</v>
+        <v>0.0157933235168457</v>
       </c>
       <c r="C5" t="n">
-        <v>0.003487348556518555</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.003481626510620117</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.003158330917358398</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.002799510955810547</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.002933502197265625</v>
+        <v>0.01604771614074707</v>
       </c>
       <c r="H5" t="n">
-        <v>0.002854108810424805</v>
+        <v>0.004022598266601562</v>
       </c>
       <c r="I5" t="n">
-        <v>0.002927303314208984</v>
+        <v>0.0101161003112793</v>
       </c>
       <c r="J5" t="n">
-        <v>0.002887725830078125</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.002881526947021484</v>
+        <v>0</v>
       </c>
       <c r="L5">
         <f>AVERAGE(B5:K5)</f>
@@ -1057,34 +1057,34 @@
         <v>800</v>
       </c>
       <c r="B6" t="n">
-        <v>0.004082441329956055</v>
+        <v>0.01618456840515137</v>
       </c>
       <c r="C6" t="n">
-        <v>0.003956794738769531</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.008474349975585938</v>
+        <v>0.01617574691772461</v>
       </c>
       <c r="E6" t="n">
-        <v>0.004492044448852539</v>
+        <v>0.003621101379394531</v>
       </c>
       <c r="F6" t="n">
-        <v>0.004628181457519531</v>
+        <v>0.009146213531494141</v>
       </c>
       <c r="G6" t="n">
-        <v>0.003955841064453125</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.003919601440429688</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.004063129425048828</v>
+        <v>0.01602816581726074</v>
       </c>
       <c r="J6" t="n">
-        <v>0.004046916961669922</v>
+        <v>0.009388208389282227</v>
       </c>
       <c r="K6" t="n">
-        <v>0.003969907760620117</v>
+        <v>0.01594018936157227</v>
       </c>
       <c r="L6">
         <f>AVERAGE(B6:K6)</f>
@@ -1100,34 +1100,34 @@
         <v>1000</v>
       </c>
       <c r="B7" t="n">
-        <v>0.005184173583984375</v>
+        <v>0.01586008071899414</v>
       </c>
       <c r="C7" t="n">
-        <v>0.004668235778808594</v>
+        <v>0.01311087608337402</v>
       </c>
       <c r="D7" t="n">
-        <v>0.005610227584838867</v>
+        <v>0.01558566093444824</v>
       </c>
       <c r="E7" t="n">
-        <v>0.004596471786499023</v>
+        <v>0.01580691337585449</v>
       </c>
       <c r="F7" t="n">
-        <v>0.004528045654296875</v>
+        <v>0.01010394096374512</v>
       </c>
       <c r="G7" t="n">
-        <v>0.004647016525268555</v>
+        <v>0.01583266258239746</v>
       </c>
       <c r="H7" t="n">
-        <v>0.004456996917724609</v>
+        <v>0.0161585807800293</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00442957878112793</v>
+        <v>0.01607418060302734</v>
       </c>
       <c r="J7" t="n">
-        <v>0.005900859832763672</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.005107402801513672</v>
+        <v>0.008038997650146484</v>
       </c>
       <c r="L7">
         <f>AVERAGE(B7:K7)</f>

</xml_diff>

<commit_message>
updated algorithms.py so executable runs as expected
</commit_message>
<xml_diff>
--- a/timing_results.xlsx
+++ b/timing_results.xlsx
@@ -526,31 +526,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>4.053115844726562e-06</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1.668930053710938e-06</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.192092895507812e-06</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>7.152557373046875e-07</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>9.5367431640625e-07</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1.192092895507812e-06</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1.192092895507812e-06</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -569,34 +569,34 @@
         <v>200</v>
       </c>
       <c r="B3" t="n">
-        <v>0.05807828903198242</v>
+        <v>0.0309150218963623</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05686426162719727</v>
+        <v>0.0305478572845459</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05745244026184082</v>
+        <v>0.03055691719055176</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0593106746673584</v>
+        <v>0.03020906448364258</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05231833457946777</v>
+        <v>0.0305488109588623</v>
       </c>
       <c r="G3" t="n">
-        <v>0.05089449882507324</v>
+        <v>0.03006911277770996</v>
       </c>
       <c r="H3" t="n">
-        <v>0.07591700553894043</v>
+        <v>0.02992415428161621</v>
       </c>
       <c r="I3" t="n">
-        <v>0.04929590225219727</v>
+        <v>0.03041577339172363</v>
       </c>
       <c r="J3" t="n">
-        <v>0.05038046836853027</v>
+        <v>0.03076577186584473</v>
       </c>
       <c r="K3" t="n">
-        <v>0.05597138404846191</v>
+        <v>0.03059697151184082</v>
       </c>
       <c r="L3">
         <f>AVERAGE(B3:K3)</f>
@@ -612,34 +612,34 @@
         <v>400</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2040259838104248</v>
+        <v>0.1229166984558105</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2096037864685059</v>
+        <v>0.1217982769012451</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2194952964782715</v>
+        <v>0.1234989166259766</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2248122692108154</v>
+        <v>0.1226058006286621</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2093229293823242</v>
+        <v>0.122128963470459</v>
       </c>
       <c r="G4" t="n">
-        <v>0.221970796585083</v>
+        <v>0.1215429306030273</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2260551452636719</v>
+        <v>0.122481107711792</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2072842121124268</v>
+        <v>0.1220979690551758</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2137517929077148</v>
+        <v>0.1200308799743652</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2056353092193604</v>
+        <v>0.1220710277557373</v>
       </c>
       <c r="L4">
         <f>AVERAGE(B4:K4)</f>
@@ -655,34 +655,34 @@
         <v>600</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4634144306182861</v>
+        <v>0.2753736972808838</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4614531993865967</v>
+        <v>0.2754411697387695</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6120820045471191</v>
+        <v>0.2749412059783936</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4511904716491699</v>
+        <v>0.2752628326416016</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4643123149871826</v>
+        <v>0.2751941680908203</v>
       </c>
       <c r="G5" t="n">
-        <v>0.475156307220459</v>
+        <v>0.2751648426055908</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5719192028045654</v>
+        <v>0.2753369808197021</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4635899066925049</v>
+        <v>0.2754991054534912</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4749021530151367</v>
+        <v>0.2758429050445557</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4656960964202881</v>
+        <v>0.2750437259674072</v>
       </c>
       <c r="L5">
         <f>AVERAGE(B5:K5)</f>
@@ -698,34 +698,34 @@
         <v>800</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8650112152099609</v>
+        <v>0.4896650314331055</v>
       </c>
       <c r="C6" t="n">
-        <v>0.82700514793396</v>
+        <v>0.4875490665435791</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9095418453216553</v>
+        <v>0.4903149604797363</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9233608245849609</v>
+        <v>0.4904420375823975</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8982982635498047</v>
+        <v>0.5159029960632324</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9550714492797852</v>
+        <v>0.4982709884643555</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8983595371246338</v>
+        <v>0.495732307434082</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9080491065979004</v>
+        <v>0.4890170097351074</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9102048873901367</v>
+        <v>0.5028071403503418</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9253726005554199</v>
+        <v>0.4872691631317139</v>
       </c>
       <c r="L6">
         <f>AVERAGE(B6:K6)</f>
@@ -741,34 +741,34 @@
         <v>1000</v>
       </c>
       <c r="B7" t="n">
-        <v>1.434290409088135</v>
+        <v>0.7674758434295654</v>
       </c>
       <c r="C7" t="n">
-        <v>1.415933132171631</v>
+        <v>0.7678558826446533</v>
       </c>
       <c r="D7" t="n">
-        <v>1.590587615966797</v>
+        <v>0.7687680721282959</v>
       </c>
       <c r="E7" t="n">
-        <v>1.633319854736328</v>
+        <v>0.7694649696350098</v>
       </c>
       <c r="F7" t="n">
-        <v>1.539464712142944</v>
+        <v>0.7703948020935059</v>
       </c>
       <c r="G7" t="n">
-        <v>1.50659441947937</v>
+        <v>0.761646032333374</v>
       </c>
       <c r="H7" t="n">
-        <v>1.43195104598999</v>
+        <v>0.769169807434082</v>
       </c>
       <c r="I7" t="n">
-        <v>1.413079023361206</v>
+        <v>0.7703900337219238</v>
       </c>
       <c r="J7" t="n">
-        <v>1.379208087921143</v>
+        <v>0.757706880569458</v>
       </c>
       <c r="K7" t="n">
-        <v>1.407622098922729</v>
+        <v>0.7794570922851562</v>
       </c>
       <c r="L7">
         <f>AVERAGE(B7:K7)</f>
@@ -885,34 +885,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>3.290176391601562e-05</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>9.059906005859375e-06</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>4.053115844726562e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2.86102294921875e-06</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>3.099441528320312e-06</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1.9073486328125e-06</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1.9073486328125e-06</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>2.145767211914062e-06</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1.668930053710938e-06</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>2.145767211914062e-06</v>
       </c>
       <c r="L2">
         <f>AVERAGE(B2:K2)</f>
@@ -928,34 +928,34 @@
         <v>200</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.001395940780639648</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.001183032989501953</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.001260995864868164</v>
       </c>
       <c r="E3" t="n">
-        <v>0.005215883255004883</v>
+        <v>0.001319169998168945</v>
       </c>
       <c r="F3" t="n">
-        <v>0.008206605911254883</v>
+        <v>0.001292705535888672</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.001212120056152344</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00806427001953125</v>
+        <v>0.001235008239746094</v>
       </c>
       <c r="I3" t="n">
-        <v>0.006873846054077148</v>
+        <v>0.001299858093261719</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>0.001294136047363281</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>0.001221895217895508</v>
       </c>
       <c r="L3">
         <f>AVERAGE(B3:K3)</f>
@@ -971,34 +971,34 @@
         <v>400</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.00265812873840332</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.002577781677246094</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01570534706115723</v>
+        <v>0.002562761306762695</v>
       </c>
       <c r="E4" t="n">
-        <v>0.009578466415405273</v>
+        <v>0.002596139907836914</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.002532243728637695</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.002537965774536133</v>
       </c>
       <c r="H4" t="n">
-        <v>0.003987550735473633</v>
+        <v>0.002564191818237305</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>0.002683162689208984</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>0.002639055252075195</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>0.002562046051025391</v>
       </c>
       <c r="L4">
         <f>AVERAGE(B4:K4)</f>
@@ -1014,34 +1014,34 @@
         <v>600</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0157933235168457</v>
+        <v>0.003829002380371094</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.003823757171630859</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.003704071044921875</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.003737688064575195</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.003611326217651367</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01604771614074707</v>
+        <v>0.003628015518188477</v>
       </c>
       <c r="H5" t="n">
-        <v>0.004022598266601562</v>
+        <v>0.003867864608764648</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0101161003112793</v>
+        <v>0.003838062286376953</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>0.003657102584838867</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>0.003650188446044922</v>
       </c>
       <c r="L5">
         <f>AVERAGE(B5:K5)</f>
@@ -1057,34 +1057,34 @@
         <v>800</v>
       </c>
       <c r="B6" t="n">
-        <v>0.01618456840515137</v>
+        <v>0.005367040634155273</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.00555109977722168</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01617574691772461</v>
+        <v>0.005207061767578125</v>
       </c>
       <c r="E6" t="n">
-        <v>0.003621101379394531</v>
+        <v>0.005244016647338867</v>
       </c>
       <c r="F6" t="n">
-        <v>0.009146213531494141</v>
+        <v>0.005380868911743164</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.005351066589355469</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.005272865295410156</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01602816581726074</v>
+        <v>0.005443096160888672</v>
       </c>
       <c r="J6" t="n">
-        <v>0.009388208389282227</v>
+        <v>0.005643606185913086</v>
       </c>
       <c r="K6" t="n">
-        <v>0.01594018936157227</v>
+        <v>0.005290985107421875</v>
       </c>
       <c r="L6">
         <f>AVERAGE(B6:K6)</f>
@@ -1100,34 +1100,34 @@
         <v>1000</v>
       </c>
       <c r="B7" t="n">
-        <v>0.01586008071899414</v>
+        <v>0.005908012390136719</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01311087608337402</v>
+        <v>0.006090879440307617</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01558566093444824</v>
+        <v>0.005795001983642578</v>
       </c>
       <c r="E7" t="n">
-        <v>0.01580691337585449</v>
+        <v>0.005869865417480469</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01010394096374512</v>
+        <v>0.005669116973876953</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01583266258239746</v>
+        <v>0.005852937698364258</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0161585807800293</v>
+        <v>0.005935907363891602</v>
       </c>
       <c r="I7" t="n">
-        <v>0.01607418060302734</v>
+        <v>0.005820989608764648</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>0.005738019943237305</v>
       </c>
       <c r="K7" t="n">
-        <v>0.008038997650146484</v>
+        <v>0.005735158920288086</v>
       </c>
       <c r="L7">
         <f>AVERAGE(B7:K7)</f>

</xml_diff>

<commit_message>
updated with Ina's code from main. Changed tests and graphs to test for more sizes. Regraphed and created executable
</commit_message>
<xml_diff>
--- a/timing_results.xlsx
+++ b/timing_results.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,34 +526,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4.053115844726562e-06</v>
+        <v>3.576278686523438e-06</v>
       </c>
       <c r="C2" t="n">
-        <v>1.668930053710938e-06</v>
+        <v>1.478195190429688e-05</v>
       </c>
       <c r="D2" t="n">
         <v>1.192092895507812e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>9.5367431640625e-07</v>
       </c>
       <c r="F2" t="n">
-        <v>7.152557373046875e-07</v>
+        <v>1.192092895507812e-06</v>
       </c>
       <c r="G2" t="n">
         <v>9.5367431640625e-07</v>
       </c>
       <c r="H2" t="n">
-        <v>1.192092895507812e-06</v>
+        <v>7.152557373046875e-07</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>7.152557373046875e-07</v>
       </c>
       <c r="J2" t="n">
-        <v>1.192092895507812e-06</v>
+        <v>2.622604370117188e-06</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>2.384185791015625e-06</v>
       </c>
       <c r="L2">
         <f>AVERAGE(B2:K2)</f>
@@ -566,37 +566,37 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0309150218963623</v>
+        <v>0.002595901489257812</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0305478572845459</v>
+        <v>0.002419233322143555</v>
       </c>
       <c r="D3" t="n">
-        <v>0.03055691719055176</v>
+        <v>0.002533435821533203</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03020906448364258</v>
+        <v>0.002760887145996094</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0305488109588623</v>
+        <v>0.002789497375488281</v>
       </c>
       <c r="G3" t="n">
-        <v>0.03006911277770996</v>
+        <v>0.002676010131835938</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02992415428161621</v>
+        <v>0.002419471740722656</v>
       </c>
       <c r="I3" t="n">
-        <v>0.03041577339172363</v>
+        <v>0.002909660339355469</v>
       </c>
       <c r="J3" t="n">
-        <v>0.03076577186584473</v>
+        <v>0.002492189407348633</v>
       </c>
       <c r="K3" t="n">
-        <v>0.03059697151184082</v>
+        <v>0.002468585968017578</v>
       </c>
       <c r="L3">
         <f>AVERAGE(B3:K3)</f>
@@ -609,37 +609,37 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1229166984558105</v>
+        <v>0.01061725616455078</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1217982769012451</v>
+        <v>0.01631331443786621</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1234989166259766</v>
+        <v>0.00970458984375</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1226058006286621</v>
+        <v>0.009839057922363281</v>
       </c>
       <c r="F4" t="n">
-        <v>0.122128963470459</v>
+        <v>0.009581089019775391</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1215429306030273</v>
+        <v>0.01037478446960449</v>
       </c>
       <c r="H4" t="n">
-        <v>0.122481107711792</v>
+        <v>0.01018381118774414</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1220979690551758</v>
+        <v>0.009801387786865234</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1200308799743652</v>
+        <v>0.01181125640869141</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1220710277557373</v>
+        <v>0.009929895401000977</v>
       </c>
       <c r="L4">
         <f>AVERAGE(B4:K4)</f>
@@ -652,37 +652,37 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2753736972808838</v>
+        <v>0.04105210304260254</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2754411697387695</v>
+        <v>0.03879523277282715</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2749412059783936</v>
+        <v>0.03829789161682129</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2752628326416016</v>
+        <v>0.04174900054931641</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2751941680908203</v>
+        <v>0.03918337821960449</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2751648426055908</v>
+        <v>0.03902482986450195</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2753369808197021</v>
+        <v>0.04598879814147949</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2754991054534912</v>
+        <v>0.0411827564239502</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2758429050445557</v>
+        <v>0.04018115997314453</v>
       </c>
       <c r="K5" t="n">
-        <v>0.2750437259674072</v>
+        <v>0.03961968421936035</v>
       </c>
       <c r="L5">
         <f>AVERAGE(B5:K5)</f>
@@ -695,37 +695,37 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4896650314331055</v>
+        <v>0.1662888526916504</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4875490665435791</v>
+        <v>0.1552770137786865</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4903149604797363</v>
+        <v>0.1603591442108154</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4904420375823975</v>
+        <v>0.1553127765655518</v>
       </c>
       <c r="F6" t="n">
-        <v>0.5159029960632324</v>
+        <v>0.1591179370880127</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4982709884643555</v>
+        <v>0.1521799564361572</v>
       </c>
       <c r="H6" t="n">
-        <v>0.495732307434082</v>
+        <v>0.1610879898071289</v>
       </c>
       <c r="I6" t="n">
-        <v>0.4890170097351074</v>
+        <v>0.1527466773986816</v>
       </c>
       <c r="J6" t="n">
-        <v>0.5028071403503418</v>
+        <v>0.1621439456939697</v>
       </c>
       <c r="K6" t="n">
-        <v>0.4872691631317139</v>
+        <v>0.1549711227416992</v>
       </c>
       <c r="L6">
         <f>AVERAGE(B6:K6)</f>
@@ -738,37 +738,37 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="B7" t="n">
-        <v>0.7674758434295654</v>
+        <v>0.6237304210662842</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7678558826446533</v>
+        <v>0.6273961067199707</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7687680721282959</v>
+        <v>0.6390266418457031</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7694649696350098</v>
+        <v>0.6265377998352051</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7703948020935059</v>
+        <v>0.6328692436218262</v>
       </c>
       <c r="G7" t="n">
-        <v>0.761646032333374</v>
+        <v>0.6343848705291748</v>
       </c>
       <c r="H7" t="n">
-        <v>0.769169807434082</v>
+        <v>0.6299924850463867</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7703900337219238</v>
+        <v>0.6288118362426758</v>
       </c>
       <c r="J7" t="n">
-        <v>0.757706880569458</v>
+        <v>0.6270408630371094</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7794570922851562</v>
+        <v>0.6495654582977295</v>
       </c>
       <c r="L7">
         <f>AVERAGE(B7:K7)</f>
@@ -776,6 +776,135 @@
       </c>
       <c r="M7">
         <f>STDEV.S(B7:K7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2.225206613540649</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.229511737823486</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.23875880241394</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2.249152660369873</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2.250405311584473</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.228482961654663</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.313826560974121</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2.272916316986084</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2.275491237640381</v>
+      </c>
+      <c r="K8" t="n">
+        <v>2.26696252822876</v>
+      </c>
+      <c r="L8">
+        <f>AVERAGE(B8:K8)</f>
+        <v/>
+      </c>
+      <c r="M8">
+        <f>STDEV.S(B8:K8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3.975231170654297</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3.972332715988159</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3.961799144744873</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.969098567962646</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3.973695039749146</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3.962504386901855</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3.982734441757202</v>
+      </c>
+      <c r="I9" t="n">
+        <v>4.005683660507202</v>
+      </c>
+      <c r="J9" t="n">
+        <v>3.913738965988159</v>
+      </c>
+      <c r="K9" t="n">
+        <v>3.968324184417725</v>
+      </c>
+      <c r="L9">
+        <f>AVERAGE(B9:K9)</f>
+        <v/>
+      </c>
+      <c r="M9">
+        <f>STDEV.S(B9:K9)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>3000</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8.802835464477539</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8.894636154174805</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8.744202852249146</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8.808440923690796</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8.718207359313965</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8.659956455230713</v>
+      </c>
+      <c r="H10" t="n">
+        <v>8.921866178512573</v>
+      </c>
+      <c r="I10" t="n">
+        <v>8.795485019683838</v>
+      </c>
+      <c r="J10" t="n">
+        <v>9.055953502655029</v>
+      </c>
+      <c r="K10" t="n">
+        <v>8.869661808013916</v>
+      </c>
+      <c r="L10">
+        <f>AVERAGE(B10:K10)</f>
+        <v/>
+      </c>
+      <c r="M10">
+        <f>STDEV.S(B10:K10)</f>
         <v/>
       </c>
     </row>
@@ -790,7 +919,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -885,34 +1014,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3.290176391601562e-05</v>
+        <v>3.337860107421875e-05</v>
       </c>
       <c r="C2" t="n">
-        <v>9.059906005859375e-06</v>
+        <v>3.24249267578125e-05</v>
       </c>
       <c r="D2" t="n">
-        <v>4.053115844726562e-06</v>
+        <v>6.437301635742188e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>2.86102294921875e-06</v>
+        <v>5.483627319335938e-06</v>
       </c>
       <c r="F2" t="n">
-        <v>3.099441528320312e-06</v>
+        <v>5.483627319335938e-06</v>
       </c>
       <c r="G2" t="n">
-        <v>1.9073486328125e-06</v>
+        <v>5.245208740234375e-06</v>
       </c>
       <c r="H2" t="n">
-        <v>1.9073486328125e-06</v>
+        <v>4.529953002929688e-06</v>
       </c>
       <c r="I2" t="n">
-        <v>2.145767211914062e-06</v>
+        <v>4.529953002929688e-06</v>
       </c>
       <c r="J2" t="n">
-        <v>1.668930053710938e-06</v>
+        <v>2.455711364746094e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>2.145767211914062e-06</v>
+        <v>1.478195190429688e-05</v>
       </c>
       <c r="L2">
         <f>AVERAGE(B2:K2)</f>
@@ -925,37 +1054,37 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="B3" t="n">
-        <v>0.001395940780639648</v>
+        <v>0.0003829002380371094</v>
       </c>
       <c r="C3" t="n">
-        <v>0.001183032989501953</v>
+        <v>0.0003759860992431641</v>
       </c>
       <c r="D3" t="n">
-        <v>0.001260995864868164</v>
+        <v>0.0003404617309570312</v>
       </c>
       <c r="E3" t="n">
-        <v>0.001319169998168945</v>
+        <v>0.0003790855407714844</v>
       </c>
       <c r="F3" t="n">
-        <v>0.001292705535888672</v>
+        <v>0.0004532337188720703</v>
       </c>
       <c r="G3" t="n">
-        <v>0.001212120056152344</v>
+        <v>0.000457763671875</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001235008239746094</v>
+        <v>0.000453948974609375</v>
       </c>
       <c r="I3" t="n">
-        <v>0.001299858093261719</v>
+        <v>0.000308990478515625</v>
       </c>
       <c r="J3" t="n">
-        <v>0.001294136047363281</v>
+        <v>0.0003244876861572266</v>
       </c>
       <c r="K3" t="n">
-        <v>0.001221895217895508</v>
+        <v>0.0003771781921386719</v>
       </c>
       <c r="L3">
         <f>AVERAGE(B3:K3)</f>
@@ -968,37 +1097,37 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="B4" t="n">
-        <v>0.00265812873840332</v>
+        <v>0.0006780624389648438</v>
       </c>
       <c r="C4" t="n">
-        <v>0.002577781677246094</v>
+        <v>0.0007014274597167969</v>
       </c>
       <c r="D4" t="n">
-        <v>0.002562761306762695</v>
+        <v>0.0006437301635742188</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002596139907836914</v>
+        <v>0.0007040500640869141</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002532243728637695</v>
+        <v>0.0007100105285644531</v>
       </c>
       <c r="G4" t="n">
-        <v>0.002537965774536133</v>
+        <v>0.000789642333984375</v>
       </c>
       <c r="H4" t="n">
-        <v>0.002564191818237305</v>
+        <v>0.0006978511810302734</v>
       </c>
       <c r="I4" t="n">
-        <v>0.002683162689208984</v>
+        <v>0.0007014274597167969</v>
       </c>
       <c r="J4" t="n">
-        <v>0.002639055252075195</v>
+        <v>0.0006926059722900391</v>
       </c>
       <c r="K4" t="n">
-        <v>0.002562046051025391</v>
+        <v>0.0006880760192871094</v>
       </c>
       <c r="L4">
         <f>AVERAGE(B4:K4)</f>
@@ -1011,37 +1140,37 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="B5" t="n">
-        <v>0.003829002380371094</v>
+        <v>0.001419305801391602</v>
       </c>
       <c r="C5" t="n">
-        <v>0.003823757171630859</v>
+        <v>0.001399993896484375</v>
       </c>
       <c r="D5" t="n">
-        <v>0.003704071044921875</v>
+        <v>0.001376867294311523</v>
       </c>
       <c r="E5" t="n">
-        <v>0.003737688064575195</v>
+        <v>0.001477241516113281</v>
       </c>
       <c r="F5" t="n">
-        <v>0.003611326217651367</v>
+        <v>0.00134587287902832</v>
       </c>
       <c r="G5" t="n">
-        <v>0.003628015518188477</v>
+        <v>0.001365900039672852</v>
       </c>
       <c r="H5" t="n">
-        <v>0.003867864608764648</v>
+        <v>0.001585721969604492</v>
       </c>
       <c r="I5" t="n">
-        <v>0.003838062286376953</v>
+        <v>0.001375675201416016</v>
       </c>
       <c r="J5" t="n">
-        <v>0.003657102584838867</v>
+        <v>0.001415491104125977</v>
       </c>
       <c r="K5" t="n">
-        <v>0.003650188446044922</v>
+        <v>0.001445531845092773</v>
       </c>
       <c r="L5">
         <f>AVERAGE(B5:K5)</f>
@@ -1054,37 +1183,37 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="B6" t="n">
-        <v>0.005367040634155273</v>
+        <v>0.002962589263916016</v>
       </c>
       <c r="C6" t="n">
-        <v>0.00555109977722168</v>
+        <v>0.003128767013549805</v>
       </c>
       <c r="D6" t="n">
-        <v>0.005207061767578125</v>
+        <v>0.003047466278076172</v>
       </c>
       <c r="E6" t="n">
-        <v>0.005244016647338867</v>
+        <v>0.002901315689086914</v>
       </c>
       <c r="F6" t="n">
-        <v>0.005380868911743164</v>
+        <v>0.002819299697875977</v>
       </c>
       <c r="G6" t="n">
-        <v>0.005351066589355469</v>
+        <v>0.002986431121826172</v>
       </c>
       <c r="H6" t="n">
-        <v>0.005272865295410156</v>
+        <v>0.002939224243164062</v>
       </c>
       <c r="I6" t="n">
-        <v>0.005443096160888672</v>
+        <v>0.002996444702148438</v>
       </c>
       <c r="J6" t="n">
-        <v>0.005643606185913086</v>
+        <v>0.003011941909790039</v>
       </c>
       <c r="K6" t="n">
-        <v>0.005290985107421875</v>
+        <v>0.002924442291259766</v>
       </c>
       <c r="L6">
         <f>AVERAGE(B6:K6)</f>
@@ -1097,37 +1226,37 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="B7" t="n">
-        <v>0.005908012390136719</v>
+        <v>0.006684064865112305</v>
       </c>
       <c r="C7" t="n">
-        <v>0.006090879440307617</v>
+        <v>0.007087945938110352</v>
       </c>
       <c r="D7" t="n">
-        <v>0.005795001983642578</v>
+        <v>0.006383895874023438</v>
       </c>
       <c r="E7" t="n">
-        <v>0.005869865417480469</v>
+        <v>0.006432294845581055</v>
       </c>
       <c r="F7" t="n">
-        <v>0.005669116973876953</v>
+        <v>0.01158452033996582</v>
       </c>
       <c r="G7" t="n">
-        <v>0.005852937698364258</v>
+        <v>0.00627589225769043</v>
       </c>
       <c r="H7" t="n">
-        <v>0.005935907363891602</v>
+        <v>0.009986639022827148</v>
       </c>
       <c r="I7" t="n">
-        <v>0.005820989608764648</v>
+        <v>0.006769418716430664</v>
       </c>
       <c r="J7" t="n">
-        <v>0.005738019943237305</v>
+        <v>0.006601333618164062</v>
       </c>
       <c r="K7" t="n">
-        <v>0.005735158920288086</v>
+        <v>0.00649714469909668</v>
       </c>
       <c r="L7">
         <f>AVERAGE(B7:K7)</f>
@@ -1135,6 +1264,135 @@
       </c>
       <c r="M7">
         <f>STDEV.S(B7:K7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.01241207122802734</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.01237297058105469</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.01250886917114258</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.01244688034057617</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0126035213470459</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.01221227645874023</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.01272058486938477</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.01233100891113281</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.01273536682128906</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.01286482810974121</v>
+      </c>
+      <c r="L8">
+        <f>AVERAGE(B8:K8)</f>
+        <v/>
+      </c>
+      <c r="M8">
+        <f>STDEV.S(B8:K8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.01806426048278809</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.01550960540771484</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.01892495155334473</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.01992130279541016</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.01701784133911133</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0198369026184082</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.01735615730285645</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.01679754257202148</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.01778006553649902</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.01632046699523926</v>
+      </c>
+      <c r="L9">
+        <f>AVERAGE(B9:K9)</f>
+        <v/>
+      </c>
+      <c r="M9">
+        <f>STDEV.S(B9:K9)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>3000</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.02908515930175781</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.02730035781860352</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.02657079696655273</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.02612066268920898</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.02603816986083984</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.02605795860290527</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.02683424949645996</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.02833366394042969</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.02717375755310059</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.02778482437133789</v>
+      </c>
+      <c r="L10">
+        <f>AVERAGE(B10:K10)</f>
+        <v/>
+      </c>
+      <c r="M10">
+        <f>STDEV.S(B10:K10)</f>
         <v/>
       </c>
     </row>
@@ -1149,7 +1407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1224,7 +1482,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <f>'Brute Force'!L3</f>
@@ -1249,7 +1507,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="B4">
         <f>'Brute Force'!L4</f>
@@ -1274,7 +1532,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="B5">
         <f>'Brute Force'!L5</f>
@@ -1299,7 +1557,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="B6">
         <f>'Brute Force'!L6</f>
@@ -1324,7 +1582,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="B7">
         <f>'Brute Force'!L7</f>
@@ -1344,6 +1602,81 @@
       </c>
       <c r="F7">
         <f>B7/D7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B8">
+        <f>'Brute Force'!L8</f>
+        <v/>
+      </c>
+      <c r="C8">
+        <f>'Brute Force'!M8</f>
+        <v/>
+      </c>
+      <c r="D8">
+        <f>'Divide and Conquer'!L8</f>
+        <v/>
+      </c>
+      <c r="E8">
+        <f>'Divide and Conquer'!M8</f>
+        <v/>
+      </c>
+      <c r="F8">
+        <f>B8/D8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B9">
+        <f>'Brute Force'!L9</f>
+        <v/>
+      </c>
+      <c r="C9">
+        <f>'Brute Force'!M9</f>
+        <v/>
+      </c>
+      <c r="D9">
+        <f>'Divide and Conquer'!L9</f>
+        <v/>
+      </c>
+      <c r="E9">
+        <f>'Divide and Conquer'!M9</f>
+        <v/>
+      </c>
+      <c r="F9">
+        <f>B9/D9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>3000</v>
+      </c>
+      <c r="B10">
+        <f>'Brute Force'!L10</f>
+        <v/>
+      </c>
+      <c r="C10">
+        <f>'Brute Force'!M10</f>
+        <v/>
+      </c>
+      <c r="D10">
+        <f>'Divide and Conquer'!L10</f>
+        <v/>
+      </c>
+      <c r="E10">
+        <f>'Divide and Conquer'!M10</f>
+        <v/>
+      </c>
+      <c r="F10">
+        <f>B10/D10</f>
         <v/>
       </c>
     </row>

</xml_diff>